<commit_message>
add lưu tiến độ
</commit_message>
<xml_diff>
--- a/Đo_An/HoanThanhDangNhap/bin/Debug/Resources/Du lieu cau hoi/thu vien bai hoc.xlsx
+++ b/Đo_An/HoanThanhDangNhap/bin/Debug/Resources/Du lieu cau hoi/thu vien bai hoc.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Đồ Án\DO AN\Do_AN\TruaNgay18New1\student_add bai hoc\HoanThanhDangNhap\bin\Debug\Resources\Du lieu cau hoi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Đăng_Quý_UTE_K19\Dang_Quy_UTE_k19\Đo_An\HoanThanhDangNhap\bin\Debug\Resources\Du lieu cau hoi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8C78870-A838-4F23-A310-36AB0B02AB40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C79D10D1-2361-47FB-A4B9-4FA4F241A1EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="9" r:id="rId1"/>
@@ -3311,8 +3311,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3322,7 +3322,9 @@
     <col min="4" max="4" width="255.77734375" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="8" width="12.109375" style="2"/>
     <col min="9" max="9" width="48" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="12.109375" style="2"/>
+    <col min="10" max="10" width="12.109375" style="2"/>
+    <col min="11" max="11" width="12.109375" style="2" customWidth="1"/>
+    <col min="12" max="16384" width="12.109375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
@@ -7971,7 +7973,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
     </sheetView>

</xml_diff>

<commit_message>
còn bài 9 trong phần bài học
</commit_message>
<xml_diff>
--- a/Đo_An/HoanThanhDangNhap/bin/Debug/Resources/Du lieu cau hoi/thu vien bai hoc.xlsx
+++ b/Đo_An/HoanThanhDangNhap/bin/Debug/Resources/Du lieu cau hoi/thu vien bai hoc.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Đồ án tốt nghiệp\doantn\dinh\Loz\Do_AN\TruaNgay18New1\student_add bai hoc\HoanThanhDangNhap\bin\Debug\Resources\Du lieu cau hoi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Đăng_Quý_UTE_K19\Dang_Quy_UTE_k19\Đo_An\HoanThanhDangNhap\bin\Debug\Resources\Du lieu cau hoi\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E374ED30-F9DF-4A90-80B1-793AEC5C7FB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="9" r:id="rId1"/>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2745" uniqueCount="672">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2746" uniqueCount="673">
   <si>
     <t>nActi</t>
   </si>
@@ -2843,11 +2844,14 @@
   <si>
     <t>\\Resources\\Hinh anh cac chuong\\hinh anh c5\\3.PNG</t>
   </si>
+  <si>
+    <t>ENDEND</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3092,13 +3096,13 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="8" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3415,7 +3419,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
@@ -3466,7 +3470,7 @@
       <c r="K1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="38"/>
+      <c r="M1" s="37"/>
     </row>
     <row r="2" spans="1:13" ht="207.6" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
@@ -3618,7 +3622,7 @@
       <c r="C6" s="4" t="s">
         <v>597</v>
       </c>
-      <c r="D6" s="37" t="s">
+      <c r="D6" s="36" t="s">
         <v>638</v>
       </c>
       <c r="E6" s="18" t="s">
@@ -3967,19 +3971,19 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
-    <hyperlink ref="C5" r:id="rId4"/>
-    <hyperlink ref="C6" r:id="rId5"/>
-    <hyperlink ref="C7" r:id="rId6"/>
-    <hyperlink ref="C8" r:id="rId7"/>
-    <hyperlink ref="C9" r:id="rId8"/>
-    <hyperlink ref="C10" r:id="rId9"/>
-    <hyperlink ref="C11" r:id="rId10"/>
-    <hyperlink ref="C12" r:id="rId11"/>
-    <hyperlink ref="C13" r:id="rId12"/>
-    <hyperlink ref="C14" r:id="rId13"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="C7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="C8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="C9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="C10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="C11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="C12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="C13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="C14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId14"/>
@@ -3987,7 +3991,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:P38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4042,11 +4046,11 @@
       <c r="J1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="36" t="s">
+      <c r="N1" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="36"/>
-      <c r="P1" s="36"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="38"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -4082,10 +4086,10 @@
       <c r="N2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="O2" s="36" t="s">
+      <c r="O2" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="36"/>
+      <c r="P2" s="38"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
@@ -4121,10 +4125,10 @@
       <c r="N3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="O3" s="36" t="s">
+      <c r="O3" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="P3" s="36"/>
+      <c r="P3" s="38"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
@@ -4160,10 +4164,10 @@
       <c r="N4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="O4" s="36" t="s">
+      <c r="O4" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="P4" s="36"/>
+      <c r="P4" s="38"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
@@ -5238,13 +5242,13 @@
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" display="\\Resources\\hinh anh c6\\relay working animation.gif"/>
-    <hyperlink ref="B7" r:id="rId2" display="\\Resources\\hinh anh c6\\relay working animation.gif"/>
-    <hyperlink ref="B10" r:id="rId3" display="\\Resources\\mach c6.png"/>
-    <hyperlink ref="B11" r:id="rId4" display="\\Resources\\mach c6.png"/>
-    <hyperlink ref="B12" r:id="rId5" display="\\Resources\\mach c6.png"/>
-    <hyperlink ref="B8" r:id="rId6" display="\\Resources\\hinh anh c6\\relay working animation.gif"/>
-    <hyperlink ref="B9" r:id="rId7" display="\\Resources\\hinh anh c6\\relay working animation.gif"/>
+    <hyperlink ref="B6" r:id="rId1" display="\\Resources\\hinh anh c6\\relay working animation.gif" xr:uid="{00000000-0004-0000-0900-000000000000}"/>
+    <hyperlink ref="B7" r:id="rId2" display="\\Resources\\hinh anh c6\\relay working animation.gif" xr:uid="{00000000-0004-0000-0900-000001000000}"/>
+    <hyperlink ref="B10" r:id="rId3" display="\\Resources\\mach c6.png" xr:uid="{00000000-0004-0000-0900-000002000000}"/>
+    <hyperlink ref="B11" r:id="rId4" display="\\Resources\\mach c6.png" xr:uid="{00000000-0004-0000-0900-000003000000}"/>
+    <hyperlink ref="B12" r:id="rId5" display="\\Resources\\mach c6.png" xr:uid="{00000000-0004-0000-0900-000004000000}"/>
+    <hyperlink ref="B8" r:id="rId6" display="\\Resources\\hinh anh c6\\relay working animation.gif" xr:uid="{00000000-0004-0000-0900-000005000000}"/>
+    <hyperlink ref="B9" r:id="rId7" display="\\Resources\\hinh anh c6\\relay working animation.gif" xr:uid="{00000000-0004-0000-0900-000006000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId8"/>
@@ -5252,7 +5256,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6390,30 +6394,30 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1"/>
-    <hyperlink ref="C5" r:id="rId2"/>
-    <hyperlink ref="C6" r:id="rId3"/>
-    <hyperlink ref="C7" r:id="rId4"/>
-    <hyperlink ref="C9" r:id="rId5"/>
-    <hyperlink ref="C10" r:id="rId6"/>
-    <hyperlink ref="C12" r:id="rId7"/>
-    <hyperlink ref="C11" r:id="rId8"/>
-    <hyperlink ref="C13" r:id="rId9"/>
-    <hyperlink ref="C14" r:id="rId10"/>
-    <hyperlink ref="C15" r:id="rId11"/>
-    <hyperlink ref="C16" r:id="rId12"/>
-    <hyperlink ref="C18" r:id="rId13"/>
-    <hyperlink ref="C19" r:id="rId14"/>
-    <hyperlink ref="C20" r:id="rId15"/>
-    <hyperlink ref="C21" r:id="rId16"/>
-    <hyperlink ref="C22" r:id="rId17"/>
-    <hyperlink ref="C24" r:id="rId18"/>
-    <hyperlink ref="C25" r:id="rId19" display="\\Resources\\Hinh anh cac chuong\\hinh anh c5\\short2ground.png"/>
-    <hyperlink ref="C30" r:id="rId20"/>
-    <hyperlink ref="C31" r:id="rId21"/>
-    <hyperlink ref="C32" r:id="rId22"/>
-    <hyperlink ref="C33" r:id="rId23"/>
-    <hyperlink ref="C2" r:id="rId24"/>
+    <hyperlink ref="C4" r:id="rId1" xr:uid="{00000000-0004-0000-0A00-000000000000}"/>
+    <hyperlink ref="C5" r:id="rId2" xr:uid="{00000000-0004-0000-0A00-000001000000}"/>
+    <hyperlink ref="C6" r:id="rId3" xr:uid="{00000000-0004-0000-0A00-000002000000}"/>
+    <hyperlink ref="C7" r:id="rId4" xr:uid="{00000000-0004-0000-0A00-000003000000}"/>
+    <hyperlink ref="C9" r:id="rId5" xr:uid="{00000000-0004-0000-0A00-000004000000}"/>
+    <hyperlink ref="C10" r:id="rId6" xr:uid="{00000000-0004-0000-0A00-000005000000}"/>
+    <hyperlink ref="C12" r:id="rId7" xr:uid="{00000000-0004-0000-0A00-000006000000}"/>
+    <hyperlink ref="C11" r:id="rId8" xr:uid="{00000000-0004-0000-0A00-000007000000}"/>
+    <hyperlink ref="C13" r:id="rId9" xr:uid="{00000000-0004-0000-0A00-000008000000}"/>
+    <hyperlink ref="C14" r:id="rId10" xr:uid="{00000000-0004-0000-0A00-000009000000}"/>
+    <hyperlink ref="C15" r:id="rId11" xr:uid="{00000000-0004-0000-0A00-00000A000000}"/>
+    <hyperlink ref="C16" r:id="rId12" xr:uid="{00000000-0004-0000-0A00-00000B000000}"/>
+    <hyperlink ref="C18" r:id="rId13" xr:uid="{00000000-0004-0000-0A00-00000C000000}"/>
+    <hyperlink ref="C19" r:id="rId14" xr:uid="{00000000-0004-0000-0A00-00000D000000}"/>
+    <hyperlink ref="C20" r:id="rId15" xr:uid="{00000000-0004-0000-0A00-00000E000000}"/>
+    <hyperlink ref="C21" r:id="rId16" xr:uid="{00000000-0004-0000-0A00-00000F000000}"/>
+    <hyperlink ref="C22" r:id="rId17" xr:uid="{00000000-0004-0000-0A00-000010000000}"/>
+    <hyperlink ref="C24" r:id="rId18" xr:uid="{00000000-0004-0000-0A00-000011000000}"/>
+    <hyperlink ref="C25" r:id="rId19" display="\\Resources\\Hinh anh cac chuong\\hinh anh c5\\short2ground.png" xr:uid="{00000000-0004-0000-0A00-000012000000}"/>
+    <hyperlink ref="C30" r:id="rId20" xr:uid="{00000000-0004-0000-0A00-000013000000}"/>
+    <hyperlink ref="C31" r:id="rId21" xr:uid="{00000000-0004-0000-0A00-000014000000}"/>
+    <hyperlink ref="C32" r:id="rId22" xr:uid="{00000000-0004-0000-0A00-000015000000}"/>
+    <hyperlink ref="C33" r:id="rId23" xr:uid="{00000000-0004-0000-0A00-000016000000}"/>
+    <hyperlink ref="C2" r:id="rId24" xr:uid="{00000000-0004-0000-0A00-000017000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId25"/>
@@ -6421,7 +6425,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -7121,30 +7125,30 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="B5" r:id="rId4"/>
-    <hyperlink ref="B6" r:id="rId5"/>
-    <hyperlink ref="B10" r:id="rId6"/>
-    <hyperlink ref="B11" r:id="rId7"/>
-    <hyperlink ref="B12" r:id="rId8" display="\\Resources\Hinh anh cac chuong\hinh anh c6\wiring_final.png"/>
-    <hyperlink ref="B13" r:id="rId9" display="\\Resources\Hinh anh cac chuong\hinh anh c6\wiring_final.png"/>
-    <hyperlink ref="B14" r:id="rId10"/>
-    <hyperlink ref="B15" r:id="rId11"/>
-    <hyperlink ref="B16" r:id="rId12"/>
-    <hyperlink ref="B17" r:id="rId13"/>
-    <hyperlink ref="B18" r:id="rId14"/>
-    <hyperlink ref="B19" r:id="rId15"/>
-    <hyperlink ref="B20" r:id="rId16"/>
-    <hyperlink ref="B21" r:id="rId17"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0B00-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0B00-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0B00-000002000000}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0B00-000003000000}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{00000000-0004-0000-0B00-000004000000}"/>
+    <hyperlink ref="B10" r:id="rId6" xr:uid="{00000000-0004-0000-0B00-000005000000}"/>
+    <hyperlink ref="B11" r:id="rId7" xr:uid="{00000000-0004-0000-0B00-000006000000}"/>
+    <hyperlink ref="B12" r:id="rId8" display="\\Resources\Hinh anh cac chuong\hinh anh c6\wiring_final.png" xr:uid="{00000000-0004-0000-0B00-000007000000}"/>
+    <hyperlink ref="B13" r:id="rId9" display="\\Resources\Hinh anh cac chuong\hinh anh c6\wiring_final.png" xr:uid="{00000000-0004-0000-0B00-000008000000}"/>
+    <hyperlink ref="B14" r:id="rId10" xr:uid="{00000000-0004-0000-0B00-000009000000}"/>
+    <hyperlink ref="B15" r:id="rId11" xr:uid="{00000000-0004-0000-0B00-00000A000000}"/>
+    <hyperlink ref="B16" r:id="rId12" xr:uid="{00000000-0004-0000-0B00-00000B000000}"/>
+    <hyperlink ref="B17" r:id="rId13" xr:uid="{00000000-0004-0000-0B00-00000C000000}"/>
+    <hyperlink ref="B18" r:id="rId14" xr:uid="{00000000-0004-0000-0B00-00000D000000}"/>
+    <hyperlink ref="B19" r:id="rId15" xr:uid="{00000000-0004-0000-0B00-00000E000000}"/>
+    <hyperlink ref="B20" r:id="rId16" xr:uid="{00000000-0004-0000-0B00-00000F000000}"/>
+    <hyperlink ref="B21" r:id="rId17" xr:uid="{00000000-0004-0000-0B00-000010000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
@@ -7910,24 +7914,24 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" display="\\Resources\\Hinh anh cac chuong\\hinh anh c7\\wiring_final.PNG"/>
-    <hyperlink ref="B4" r:id="rId2" display="\\Resources\\Hinh anh cac chuong\\hinh anh c7\\wiring_final.PNG"/>
-    <hyperlink ref="B6" r:id="rId3"/>
-    <hyperlink ref="B8" r:id="rId4"/>
-    <hyperlink ref="B2" r:id="rId5"/>
-    <hyperlink ref="B7" r:id="rId6"/>
-    <hyperlink ref="B11" r:id="rId7"/>
-    <hyperlink ref="B12" r:id="rId8"/>
-    <hyperlink ref="B13" r:id="rId9"/>
-    <hyperlink ref="B14" r:id="rId10"/>
-    <hyperlink ref="B15" r:id="rId11"/>
-    <hyperlink ref="B17" r:id="rId12"/>
-    <hyperlink ref="B18" r:id="rId13"/>
-    <hyperlink ref="B19" r:id="rId14"/>
-    <hyperlink ref="B20" r:id="rId15"/>
-    <hyperlink ref="B21" r:id="rId16"/>
-    <hyperlink ref="B22" r:id="rId17" display="\\Resources\\Hinh anh cac chuong\\hinh anh c7\\wiring_final.PNG"/>
-    <hyperlink ref="B23" r:id="rId18"/>
+    <hyperlink ref="B3" r:id="rId1" display="\\Resources\\Hinh anh cac chuong\\hinh anh c7\\wiring_final.PNG" xr:uid="{00000000-0004-0000-0C00-000000000000}"/>
+    <hyperlink ref="B4" r:id="rId2" display="\\Resources\\Hinh anh cac chuong\\hinh anh c7\\wiring_final.PNG" xr:uid="{00000000-0004-0000-0C00-000001000000}"/>
+    <hyperlink ref="B6" r:id="rId3" xr:uid="{00000000-0004-0000-0C00-000002000000}"/>
+    <hyperlink ref="B8" r:id="rId4" xr:uid="{00000000-0004-0000-0C00-000003000000}"/>
+    <hyperlink ref="B2" r:id="rId5" xr:uid="{00000000-0004-0000-0C00-000004000000}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{00000000-0004-0000-0C00-000005000000}"/>
+    <hyperlink ref="B11" r:id="rId7" xr:uid="{00000000-0004-0000-0C00-000006000000}"/>
+    <hyperlink ref="B12" r:id="rId8" xr:uid="{00000000-0004-0000-0C00-000007000000}"/>
+    <hyperlink ref="B13" r:id="rId9" xr:uid="{00000000-0004-0000-0C00-000008000000}"/>
+    <hyperlink ref="B14" r:id="rId10" xr:uid="{00000000-0004-0000-0C00-000009000000}"/>
+    <hyperlink ref="B15" r:id="rId11" xr:uid="{00000000-0004-0000-0C00-00000A000000}"/>
+    <hyperlink ref="B17" r:id="rId12" xr:uid="{00000000-0004-0000-0C00-00000B000000}"/>
+    <hyperlink ref="B18" r:id="rId13" xr:uid="{00000000-0004-0000-0C00-00000C000000}"/>
+    <hyperlink ref="B19" r:id="rId14" xr:uid="{00000000-0004-0000-0C00-00000D000000}"/>
+    <hyperlink ref="B20" r:id="rId15" xr:uid="{00000000-0004-0000-0C00-00000E000000}"/>
+    <hyperlink ref="B21" r:id="rId16" xr:uid="{00000000-0004-0000-0C00-00000F000000}"/>
+    <hyperlink ref="B22" r:id="rId17" display="\\Resources\\Hinh anh cac chuong\\hinh anh c7\\wiring_final.PNG" xr:uid="{00000000-0004-0000-0C00-000010000000}"/>
+    <hyperlink ref="B23" r:id="rId18" xr:uid="{00000000-0004-0000-0C00-000011000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId19"/>
@@ -7935,7 +7939,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8441,24 +8445,24 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1"/>
-    <hyperlink ref="B6" r:id="rId2"/>
-    <hyperlink ref="B7" r:id="rId3"/>
-    <hyperlink ref="B8" r:id="rId4"/>
-    <hyperlink ref="B9" r:id="rId5"/>
-    <hyperlink ref="B10" r:id="rId6"/>
-    <hyperlink ref="B11" r:id="rId7"/>
-    <hyperlink ref="B12" r:id="rId8"/>
-    <hyperlink ref="B13" r:id="rId9"/>
-    <hyperlink ref="B14" r:id="rId10"/>
-    <hyperlink ref="B15" r:id="rId11"/>
+    <hyperlink ref="B5" r:id="rId1" xr:uid="{00000000-0004-0000-0D00-000000000000}"/>
+    <hyperlink ref="B6" r:id="rId2" xr:uid="{00000000-0004-0000-0D00-000001000000}"/>
+    <hyperlink ref="B7" r:id="rId3" xr:uid="{00000000-0004-0000-0D00-000002000000}"/>
+    <hyperlink ref="B8" r:id="rId4" xr:uid="{00000000-0004-0000-0D00-000003000000}"/>
+    <hyperlink ref="B9" r:id="rId5" xr:uid="{00000000-0004-0000-0D00-000004000000}"/>
+    <hyperlink ref="B10" r:id="rId6" xr:uid="{00000000-0004-0000-0D00-000005000000}"/>
+    <hyperlink ref="B11" r:id="rId7" xr:uid="{00000000-0004-0000-0D00-000006000000}"/>
+    <hyperlink ref="B12" r:id="rId8" xr:uid="{00000000-0004-0000-0D00-000007000000}"/>
+    <hyperlink ref="B13" r:id="rId9" xr:uid="{00000000-0004-0000-0D00-000008000000}"/>
+    <hyperlink ref="B14" r:id="rId10" xr:uid="{00000000-0004-0000-0D00-000009000000}"/>
+    <hyperlink ref="B15" r:id="rId11" xr:uid="{00000000-0004-0000-0D00-00000A000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -9279,30 +9283,30 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="B5" r:id="rId4"/>
-    <hyperlink ref="B6" r:id="rId5"/>
-    <hyperlink ref="B7" r:id="rId6"/>
-    <hyperlink ref="B8" r:id="rId7"/>
-    <hyperlink ref="B9" r:id="rId8"/>
-    <hyperlink ref="B10" r:id="rId9"/>
-    <hyperlink ref="B11" r:id="rId10"/>
-    <hyperlink ref="B12" r:id="rId11"/>
-    <hyperlink ref="B13" r:id="rId12"/>
-    <hyperlink ref="B14" r:id="rId13"/>
-    <hyperlink ref="B15" r:id="rId14"/>
-    <hyperlink ref="B16" r:id="rId15"/>
-    <hyperlink ref="B17" r:id="rId16"/>
-    <hyperlink ref="B19" r:id="rId17"/>
-    <hyperlink ref="B20" r:id="rId18"/>
-    <hyperlink ref="B22" r:id="rId19"/>
-    <hyperlink ref="B23" r:id="rId20"/>
-    <hyperlink ref="B24" r:id="rId21"/>
-    <hyperlink ref="B25" r:id="rId22"/>
-    <hyperlink ref="B21" r:id="rId23"/>
-    <hyperlink ref="B18" r:id="rId24"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0E00-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0E00-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0E00-000002000000}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0E00-000003000000}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{00000000-0004-0000-0E00-000004000000}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{00000000-0004-0000-0E00-000005000000}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{00000000-0004-0000-0E00-000006000000}"/>
+    <hyperlink ref="B9" r:id="rId8" xr:uid="{00000000-0004-0000-0E00-000007000000}"/>
+    <hyperlink ref="B10" r:id="rId9" xr:uid="{00000000-0004-0000-0E00-000008000000}"/>
+    <hyperlink ref="B11" r:id="rId10" xr:uid="{00000000-0004-0000-0E00-000009000000}"/>
+    <hyperlink ref="B12" r:id="rId11" xr:uid="{00000000-0004-0000-0E00-00000A000000}"/>
+    <hyperlink ref="B13" r:id="rId12" xr:uid="{00000000-0004-0000-0E00-00000B000000}"/>
+    <hyperlink ref="B14" r:id="rId13" xr:uid="{00000000-0004-0000-0E00-00000C000000}"/>
+    <hyperlink ref="B15" r:id="rId14" xr:uid="{00000000-0004-0000-0E00-00000D000000}"/>
+    <hyperlink ref="B16" r:id="rId15" xr:uid="{00000000-0004-0000-0E00-00000E000000}"/>
+    <hyperlink ref="B17" r:id="rId16" xr:uid="{00000000-0004-0000-0E00-00000F000000}"/>
+    <hyperlink ref="B19" r:id="rId17" xr:uid="{00000000-0004-0000-0E00-000010000000}"/>
+    <hyperlink ref="B20" r:id="rId18" xr:uid="{00000000-0004-0000-0E00-000011000000}"/>
+    <hyperlink ref="B22" r:id="rId19" xr:uid="{00000000-0004-0000-0E00-000012000000}"/>
+    <hyperlink ref="B23" r:id="rId20" xr:uid="{00000000-0004-0000-0E00-000013000000}"/>
+    <hyperlink ref="B24" r:id="rId21" xr:uid="{00000000-0004-0000-0E00-000014000000}"/>
+    <hyperlink ref="B25" r:id="rId22" xr:uid="{00000000-0004-0000-0E00-000015000000}"/>
+    <hyperlink ref="B21" r:id="rId23" xr:uid="{00000000-0004-0000-0E00-000016000000}"/>
+    <hyperlink ref="B18" r:id="rId24" xr:uid="{00000000-0004-0000-0E00-000017000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId25"/>
@@ -9310,7 +9314,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView topLeftCell="A9" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
@@ -9359,8 +9363,8 @@
       <c r="K1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
     </row>
     <row r="2" spans="1:13" ht="180" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
@@ -9825,19 +9829,19 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
-    <hyperlink ref="C5" r:id="rId4"/>
-    <hyperlink ref="C6" r:id="rId5"/>
-    <hyperlink ref="C7" r:id="rId6"/>
-    <hyperlink ref="C8" r:id="rId7"/>
-    <hyperlink ref="C9" r:id="rId8"/>
-    <hyperlink ref="C10" r:id="rId9"/>
-    <hyperlink ref="C11" r:id="rId10"/>
-    <hyperlink ref="C12" r:id="rId11"/>
-    <hyperlink ref="C13" r:id="rId12"/>
-    <hyperlink ref="C14" r:id="rId13"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="C7" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="C8" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="C9" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="C10" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="C11" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="C12" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
+    <hyperlink ref="C13" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
+    <hyperlink ref="C14" r:id="rId13" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId14"/>
@@ -9845,7 +9849,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView zoomScale="106" zoomScaleNormal="68" workbookViewId="0">
@@ -10053,10 +10057,10 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
-    <hyperlink ref="C5" r:id="rId4"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
@@ -10064,7 +10068,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
@@ -10380,24 +10384,24 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
-    <hyperlink ref="C5" r:id="rId4"/>
-    <hyperlink ref="C6" r:id="rId5"/>
-    <hyperlink ref="C7" r:id="rId6"/>
-    <hyperlink ref="C8" r:id="rId7"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
+    <hyperlink ref="C7" r:id="rId6" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
+    <hyperlink ref="C8" r:id="rId7" xr:uid="{00000000-0004-0000-0300-000006000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10552,19 +10556,22 @@
       <c r="A5" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="B5" s="2" t="s">
+        <v>672</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
@@ -10866,13 +10873,13 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="\\Resources\mach trang.jpg"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
-    <hyperlink ref="C5" r:id="rId4"/>
-    <hyperlink ref="C6" r:id="rId5"/>
-    <hyperlink ref="C7" r:id="rId6"/>
-    <hyperlink ref="C8" r:id="rId7"/>
+    <hyperlink ref="C2" r:id="rId1" display="\\Resources\mach trang.jpg" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{00000000-0004-0000-0500-000003000000}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{00000000-0004-0000-0500-000004000000}"/>
+    <hyperlink ref="C7" r:id="rId6" xr:uid="{00000000-0004-0000-0500-000005000000}"/>
+    <hyperlink ref="C8" r:id="rId7" xr:uid="{00000000-0004-0000-0500-000006000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId8"/>
@@ -10880,10 +10887,10 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -11543,23 +11550,23 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3" display="\\Resources\mach trang.jpg"/>
-    <hyperlink ref="C5" r:id="rId4"/>
-    <hyperlink ref="C6" r:id="rId5"/>
-    <hyperlink ref="C7" r:id="rId6"/>
-    <hyperlink ref="C8" r:id="rId7"/>
-    <hyperlink ref="C9" r:id="rId8"/>
-    <hyperlink ref="C10" r:id="rId9"/>
-    <hyperlink ref="C11" r:id="rId10"/>
-    <hyperlink ref="C12" r:id="rId11" display="\\Resources\mach trang.jpg"/>
-    <hyperlink ref="C13" r:id="rId12"/>
-    <hyperlink ref="C14" r:id="rId13"/>
-    <hyperlink ref="C15" r:id="rId14"/>
-    <hyperlink ref="C16" r:id="rId15"/>
-    <hyperlink ref="C17" r:id="rId16"/>
-    <hyperlink ref="C18" r:id="rId17"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId3" display="\\Resources\mach trang.jpg" xr:uid="{00000000-0004-0000-0600-000002000000}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{00000000-0004-0000-0600-000003000000}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{00000000-0004-0000-0600-000004000000}"/>
+    <hyperlink ref="C7" r:id="rId6" xr:uid="{00000000-0004-0000-0600-000005000000}"/>
+    <hyperlink ref="C8" r:id="rId7" xr:uid="{00000000-0004-0000-0600-000006000000}"/>
+    <hyperlink ref="C9" r:id="rId8" xr:uid="{00000000-0004-0000-0600-000007000000}"/>
+    <hyperlink ref="C10" r:id="rId9" xr:uid="{00000000-0004-0000-0600-000008000000}"/>
+    <hyperlink ref="C11" r:id="rId10" xr:uid="{00000000-0004-0000-0600-000009000000}"/>
+    <hyperlink ref="C12" r:id="rId11" display="\\Resources\mach trang.jpg" xr:uid="{00000000-0004-0000-0600-00000A000000}"/>
+    <hyperlink ref="C13" r:id="rId12" xr:uid="{00000000-0004-0000-0600-00000B000000}"/>
+    <hyperlink ref="C14" r:id="rId13" xr:uid="{00000000-0004-0000-0600-00000C000000}"/>
+    <hyperlink ref="C15" r:id="rId14" xr:uid="{00000000-0004-0000-0600-00000D000000}"/>
+    <hyperlink ref="C16" r:id="rId15" xr:uid="{00000000-0004-0000-0600-00000E000000}"/>
+    <hyperlink ref="C17" r:id="rId16" xr:uid="{00000000-0004-0000-0600-00000F000000}"/>
+    <hyperlink ref="C18" r:id="rId17" xr:uid="{00000000-0004-0000-0600-000010000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId18"/>
@@ -11567,7 +11574,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12239,16 +12246,16 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="B5" r:id="rId4"/>
-    <hyperlink ref="B6" r:id="rId5"/>
-    <hyperlink ref="B14" r:id="rId6"/>
-    <hyperlink ref="B15" r:id="rId7"/>
-    <hyperlink ref="B16" r:id="rId8"/>
-    <hyperlink ref="B17" r:id="rId9"/>
-    <hyperlink ref="B18" r:id="rId10"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0700-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0700-000002000000}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0700-000003000000}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{00000000-0004-0000-0700-000004000000}"/>
+    <hyperlink ref="B14" r:id="rId6" xr:uid="{00000000-0004-0000-0700-000005000000}"/>
+    <hyperlink ref="B15" r:id="rId7" xr:uid="{00000000-0004-0000-0700-000006000000}"/>
+    <hyperlink ref="B16" r:id="rId8" xr:uid="{00000000-0004-0000-0700-000007000000}"/>
+    <hyperlink ref="B17" r:id="rId9" xr:uid="{00000000-0004-0000-0700-000008000000}"/>
+    <hyperlink ref="B18" r:id="rId10" xr:uid="{00000000-0004-0000-0700-000009000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId11"/>
@@ -12256,7 +12263,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>